<commit_message>
Updating button part number
Updated part number for button in the BoM
</commit_message>
<xml_diff>
--- a/Documentation/Open_Playback_Recorder_BOM.xlsx
+++ b/Documentation/Open_Playback_Recorder_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 22-10 Open Playback Device/Open-Playback-Recorder/Open-Playback-Recorder/Documentation/Working_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradw\GitHub\Open-Playback-Recorder\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1106" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4B11C6B-0264-4033-94D4-DD0C02933B9D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468BD287-8EE8-417E-8772-A15CED55386E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="132">
   <si>
     <t>Unit Cost</t>
   </si>
@@ -443,6 +443,9 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/duracell-industrial-operations-inc/9V/21259959</t>
+  </si>
+  <si>
+    <t>Buttons (B3F-3152)</t>
   </si>
 </sst>
 </file>
@@ -1171,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1554,7 @@
         <v>80</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -2782,13 +2785,42 @@
     <hyperlink ref="K14" r:id="rId20" xr:uid="{D451122D-1DDE-4F51-B853-9328C0136ABF}"/>
     <hyperlink ref="K15" r:id="rId21" xr:uid="{25780068-25D7-40CB-B913-2C6477D69214}"/>
     <hyperlink ref="K21" r:id="rId22" xr:uid="{1AF067E7-A776-47AD-AAFD-86DAECD9B5BB}"/>
+    <hyperlink ref="K12" r:id="rId23" xr:uid="{2033B88C-AE59-4F3F-B2C1-3D84E368DA22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B51EC7ECFAC78D4E8EF6CBAFFF0B3505" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c16a8de1b3ad07fcfe40131daee80152">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" xmlns:ns3="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85720a748046338a72a4f25fe522aa39" ns2:_="" ns3:_="">
     <xsd:import namespace="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
@@ -3037,35 +3069,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E5EB692-D7F8-4E14-B2F1-51BDE658334F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3082,23 +3105,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
-    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>